<commit_message>
Added in 4 new sheets with our names
Put in 4 new sheets each with our names on them for easy sorting
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,15 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4TaL\Desktop\School Semesters\Fall 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jjyoy\Documents\GitHubRepo\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55F1554-6E59-470D-9C4D-8E37405A1CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A5BAA-ED05-498F-BE58-B868CAFE8942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
+    <sheet name="Joseph Pak (Poducer and Design)" sheetId="2" r:id="rId2"/>
+    <sheet name="Wyatt(Artist)" sheetId="3" r:id="rId3"/>
+    <sheet name="Emanuel(designer)" sheetId="4" r:id="rId4"/>
+    <sheet name="Raphael Brown(Programmer)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Footsteps</t>
   </si>
@@ -519,16 +523,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1CC92-1BCB-4D56-BC10-E090CE41DC11}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.7265625" customWidth="1"/>
+    <col min="1" max="1" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -548,112 +552,112 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -662,4 +666,148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35965238-89E8-4AC6-982E-FD30A85DBAA4}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AABDC-3709-43B7-A9D3-19D374AE1A97}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C689EB-A68B-4BC4-B6BF-F1BC87CF5393}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added some of my Task from last semester
added my task from last semester to work on and also finished.
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\GitHub\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60AE49A-C544-4745-B54A-EF274E49CFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC99481A-4737-47BE-B8A9-294AB4174EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="12264" windowHeight="12336" tabRatio="731" firstSheet="2" activeTab="3" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="5340" yWindow="1290" windowWidth="21600" windowHeight="11385" tabRatio="731" firstSheet="1" activeTab="1" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>Footsteps</t>
   </si>
@@ -170,12 +170,60 @@
   <si>
     <t>Pause/Main Menu</t>
   </si>
+  <si>
+    <t>coding</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>respawn</t>
+  </si>
+  <si>
+    <t>Platfroms</t>
+  </si>
+  <si>
+    <t>Simple world Layout</t>
+  </si>
+  <si>
+    <t>First Area Layout</t>
+  </si>
+  <si>
+    <t>checkpoint</t>
+  </si>
+  <si>
+    <t>Background art</t>
+  </si>
+  <si>
+    <t>Platform layout</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Level tile art</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +254,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF11734B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFB10202"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF473821"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -215,7 +292,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -223,11 +300,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,6 +328,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,12 +667,12 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -582,112 +692,112 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -700,18 +810,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -731,8 +844,169 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="6">
+        <v>45033</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="6">
+        <v>44998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="6">
+        <v>44990</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="6">
+        <v>44991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="6">
+        <v>45033</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="6">
+        <v>45010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="6">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="6">
+        <v>44996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -744,9 +1018,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -776,16 +1050,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AABDC-3709-43B7-A9D3-19D374AE1A97}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -805,53 +1079,53 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
   </sheetData>
@@ -868,9 +1142,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Added some more task for me
Added task to rework the GDD and the first Level
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\GitHub\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48627C87-543C-4E21-AF7A-8BA2C5427500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04756DC-3D5E-4BF3-9379-C1CC0F8C7639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="731" firstSheet="2" activeTab="3" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="731" activeTab="1" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
   <si>
     <t>Footsteps</t>
   </si>
@@ -209,60 +209,90 @@
   </si>
   <si>
     <t>Coding</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Running Animation</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Platform Art</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Game Art</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Menu Escape</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Volume</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>High</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Not Started</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tutorial Drawings</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Low</t>
-    <phoneticPr fontId="9"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Emanuel</t>
   </si>
   <si>
     <t>N/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rework first level layout </t>
+  </si>
+  <si>
+    <t>GDD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Rework The GDD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,33 +330,44 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF11734B"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFB10202"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF473821"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="6"/>
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF11734B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB10202"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF473821"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -338,7 +379,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -361,11 +402,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,25 +427,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,7 +778,7 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
   </cols>
@@ -739,12 +803,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -850,7 +914,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -858,21 +922,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -888,172 +952,212 @@
       <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="13">
         <v>45033</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="13">
         <v>44998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="13">
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="13">
         <v>44991</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="13">
         <v>45033</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="13">
         <v>45010</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="13">
         <v>44995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="13">
         <v>44996</v>
       </c>
     </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="14">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="14">
+        <v>45178</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="9"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1063,11 +1167,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35965238-89E8-4AC6-982E-FD30A85DBAA4}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1104,7 +1208,7 @@
       <c r="E3" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="5">
         <v>45199</v>
       </c>
     </row>
@@ -1118,7 +1222,7 @@
       <c r="E4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="5">
         <v>45192</v>
       </c>
     </row>
@@ -1132,7 +1236,7 @@
       <c r="E5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="5">
         <v>45201</v>
       </c>
     </row>
@@ -1151,7 +1255,7 @@
       <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>45181</v>
       </c>
     </row>
@@ -1165,12 +1269,12 @@
       <c r="E13" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="5">
         <v>45181</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1180,14 +1284,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AABDC-3709-43B7-A9D3-19D374AE1A97}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1334,7 +1438,7 @@
       <c r="A15" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
@@ -1348,7 +1452,7 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1371,7 +1475,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished The Schedule and finalized the assets list
Finished The Schedule for my section and added some task for programmer as well as updated the full assets list
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4TaL\Desktop\School Semesters\Fall 2023\489GIT\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Desktop\Game 490 temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0B5B8-FE4B-422C-91AB-DC2413D04270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046C0304-3C16-49AC-B5F0-B542EC5994B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="731" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="270" yWindow="600" windowWidth="17355" windowHeight="13635" tabRatio="731" firstSheet="2" activeTab="2" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="125">
   <si>
     <t>Footsteps</t>
   </si>
@@ -193,10 +193,6 @@
     <t>Med</t>
   </si>
   <si>
-    <t>Coding</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Running Animation</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -324,9 +320,6 @@
     <t>Design a Save Room</t>
   </si>
   <si>
-    <t>Mini Map layout</t>
-  </si>
-  <si>
     <t xml:space="preserve">Area 1 minimap </t>
   </si>
   <si>
@@ -366,9 +359,6 @@
     <t>Area 4</t>
   </si>
   <si>
-    <t>Door with a lock and a key </t>
-  </si>
-  <si>
     <t>Lava – on the floor and on walls (are like spikes)</t>
   </si>
   <si>
@@ -390,20 +380,105 @@
     <t xml:space="preserve">Saw (likes spikes but moves) </t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Enemy hit</t>
-  </si>
-  <si>
-    <t>Draft Updated</t>
+    <t xml:space="preserve">One-way Platforms </t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Raphael Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Door with a lock and a key (check for fix) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claw wall climb. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic grab shoot </t>
+  </si>
+  <si>
+    <t>Magnetic grab box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water pump jump </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Pump shoot </t>
+  </si>
+  <si>
+    <t>Saving System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water resource (used for pump) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy resource (use for combat) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save rooms that track progress and what the player has </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check point system(For falling into pits and lava) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Magnetic grab button</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Water pump button </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dash </t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walk </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shoot player.</t>
+    </r>
+  </si>
+  <si>
+    <t>Attack player – melee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spawner (when player leaves room) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP </t>
+  </si>
+  <si>
+    <t>Enemy AI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,34 +524,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF11734B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFB10202"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF473821"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -490,6 +537,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,13 +602,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -561,38 +619,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -909,16 +959,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1CC92-1BCB-4D56-BC10-E090CE41DC11}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -929,12 +979,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.5">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.5">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -944,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -952,7 +1002,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -960,10 +1010,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="20.149999999999999" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -973,7 +1023,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -981,7 +1031,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -993,40 +1043,28 @@
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1034,43 +1072,35 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
+      <c r="A22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="B27" t="s">
         <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1082,21 +1112,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
-    <col min="2" max="2" width="37.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1112,380 +1142,732 @@
       <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="15">
         <v>45033</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="B3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="15">
         <v>44998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="15">
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="15">
         <v>44991</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="15">
         <v>45033</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="15">
         <v>45010</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="15">
         <v>44995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="15">
         <v>44996</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="16">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="14">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="16">
         <v>45182</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="F12" s="14">
-        <v>45184</v>
-      </c>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1"/>
-    <row r="15" spans="1:6" ht="15" thickBot="1">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
       <c r="A16" t="s">
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+        <v>80</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="4">
+        <v>45184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
+        <v>86</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" t="s">
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
+        <v>87</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1">
+        <v>88</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1">
+        <v>89</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1">
+        <v>81</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="4">
+        <v>45183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" t="s">
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>83</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="4">
+        <v>45192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1">
+        <v>85</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1">
       <c r="A24" t="s">
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1">
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1">
+        <v>91</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" t="s">
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1">
+        <v>92</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
       <c r="A27" t="s">
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1">
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1">
-      <c r="B29" s="19"/>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1">
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1">
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="3:3">
-      <c r="C33" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B29" s="11"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="4">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="4">
+        <v>44995</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="4">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="4">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="4">
+        <v>45188</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -1498,13 +1880,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35965238-89E8-4AC6-982E-FD30A85DBAA4}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1529,54 +1914,54 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="5">
+        <v>54</v>
+      </c>
+      <c r="F3" s="4">
         <v>45199</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>45192</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
         <v>56</v>
       </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
       <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="5">
+        <v>54</v>
+      </c>
+      <c r="F5" s="4">
         <v>45201</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -1584,68 +1969,68 @@
       <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="9">
         <v>45194</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="9">
         <v>45201</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>45181</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>45181</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
         <v>66</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="9">
         <v>45201</v>
       </c>
     </row>
@@ -1661,13 +2046,13 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D15"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1696,43 +2081,43 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
       <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1743,16 +2128,16 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1763,16 +2148,16 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1783,109 +2168,109 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
-        <v>72</v>
+      <c r="A9" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
         <v>76</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
         <v>79</v>
       </c>
-      <c r="B14" t="s">
-        <v>80</v>
-      </c>
       <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
         <v>58</v>
       </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>59</v>
-      </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>59</v>
-      </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1897,19 +2282,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C689EB-A68B-4BC4-B6BF-F1BC87CF5393}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="47.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1925,49 +2314,222 @@
       <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15">
+        <v>45033</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="B3" s="20" t="s">
+      <c r="C5" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="B4" s="20" t="s">
+      <c r="C6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="B5" s="20" t="s">
+      <c r="C7" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="20" t="s">
+      <c r="C8" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="20" t="s">
-        <v>102</v>
-      </c>
+      <c r="C9" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>

</xml_diff>

<commit_message>
Updated the Schedule for Raphael Brown and more changes
Updated the Schedule for Raphael Brown and added some more tweaks in the assets list (the programing part) and added some detail on the Hunter (in enemy and Hunter)
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\GitHub\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96771290-4CFC-4161-91A4-956111DF3ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D154D528-F17C-44E4-9C7B-86EC1AA5AB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="3" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="270" yWindow="600" windowWidth="14040" windowHeight="13635" tabRatio="731" firstSheet="2" activeTab="4" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="138">
   <si>
     <t>Footsteps</t>
   </si>
@@ -323,12 +323,6 @@
     <t>Platform moving</t>
   </si>
   <si>
-    <t>Area 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area 1 </t>
-  </si>
-  <si>
     <t>Area 2 minimap</t>
   </si>
   <si>
@@ -342,12 +336,6 @@
   </si>
   <si>
     <t xml:space="preserve">Area 2 </t>
-  </si>
-  <si>
-    <t>Area 3</t>
-  </si>
-  <si>
-    <t>Area 4</t>
   </si>
   <si>
     <t>Lava – on the floor and on walls (are like spikes)</t>
@@ -490,6 +478,39 @@
   </si>
   <si>
     <t>Player UI/ Looks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area 1 skeleton </t>
+  </si>
+  <si>
+    <t>Area 2 skeleton</t>
+  </si>
+  <si>
+    <t>Area 3 skeleton</t>
+  </si>
+  <si>
+    <t>Area 4 skeleton</t>
+  </si>
+  <si>
+    <t>Area 5 skeleton</t>
+  </si>
+  <si>
+    <t>Fix sticking to walls (ground check need to be changed.)</t>
+  </si>
+  <si>
+    <t>Area 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crates (breakable tiles but respawn when player leave room) </t>
   </si>
 </sst>
 </file>
@@ -975,10 +996,10 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -989,12 +1010,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1025,7 +1046,7 @@
     </row>
     <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1139,19 +1160,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1171,7 +1192,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
@@ -1191,7 +1212,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -1211,7 +1232,7 @@
         <v>44998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1231,7 +1252,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1251,7 +1272,7 @@
         <v>44991</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1271,7 +1292,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1291,7 +1312,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -1311,7 +1332,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1377,11 +1398,11 @@
     <row r="13" spans="1:6">
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1"/>
-    <row r="15" spans="1:6" ht="15" thickBot="1">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1395,18 +1416,18 @@
         <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F16" s="4">
         <v>45184</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>37</v>
@@ -1415,18 +1436,18 @@
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F17" s="4">
         <v>45188</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>37</v>
@@ -1441,12 +1462,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>37</v>
@@ -1461,12 +1482,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>37</v>
@@ -1481,7 +1502,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1501,7 +1522,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1512,7 +1533,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
         <v>41</v>
@@ -1526,7 +1547,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>37</v>
@@ -1535,18 +1556,18 @@
         <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="4">
         <v>45188</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1">
+    <row r="24" spans="1:8" ht="15.75" thickBot="1">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1561,12 +1582,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>37</v>
@@ -1581,12 +1602,12 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>37</v>
@@ -1601,12 +1622,12 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>37</v>
@@ -1621,19 +1642,19 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1">
       <c r="B29" s="11"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>37</v>
@@ -1648,17 +1669,17 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1">
+    <row r="32" spans="1:8" ht="15.75" thickBot="1">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
-      </c>
-      <c r="C32" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D32" t="s">
@@ -1668,18 +1689,18 @@
         <v>40</v>
       </c>
       <c r="F32" s="4">
-        <v>44995</v>
+        <v>45200</v>
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" t="s">
         <v>37</v>
       </c>
       <c r="D33" t="s">
@@ -1689,15 +1710,15 @@
         <v>41</v>
       </c>
       <c r="F33" s="4">
-        <v>45188</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>37</v>
@@ -1709,15 +1730,15 @@
         <v>41</v>
       </c>
       <c r="F34" s="4">
-        <v>45188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>37</v>
@@ -1729,15 +1750,15 @@
         <v>41</v>
       </c>
       <c r="F35" s="4">
-        <v>45195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>37</v>
@@ -1749,150 +1770,38 @@
         <v>41</v>
       </c>
       <c r="F36" s="4">
-        <v>45195</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1">
-      <c r="A37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" s="4">
-        <v>45195</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1"/>
-    <row r="39" spans="1:6" ht="15" thickBot="1">
-      <c r="A39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="4">
-        <v>44995</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F40" s="4">
-        <v>44995</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1"/>
-    <row r="42" spans="1:6" ht="15" thickBot="1">
-      <c r="A42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="4">
-        <v>45188</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1">
-      <c r="A43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="4">
-        <v>45195</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1">
-      <c r="A44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="4">
-        <v>45188</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" thickBot="1">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="4">
-        <v>45188</v>
-      </c>
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C37" s="6"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C39" s="6"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C40" s="6"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C42" s="6"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C43" s="6"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C44" s="6"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C45" s="6"/>
+      <c r="F45" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -1909,12 +1818,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2014,7 +1923,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2025,7 +1934,7 @@
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F12" s="4">
         <v>45181</v>
@@ -2039,7 +1948,7 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F13" s="4">
         <v>45181</v>
@@ -2070,16 +1979,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AABDC-3709-43B7-A9D3-19D374AE1A97}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2106,7 +2015,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -2118,12 +2027,12 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -2135,7 +2044,7 @@
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2152,7 +2061,7 @@
         <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2169,7 +2078,7 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2177,7 +2086,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -2186,7 +2095,7 @@
         <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2272,15 +2181,15 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C18" t="s">
         <v>54</v>
@@ -2294,10 +2203,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
         <v>54</v>
@@ -2318,23 +2227,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C689EB-A68B-4BC4-B6BF-F1BC87CF5393}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="50.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2354,15 +2263,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>39</v>
@@ -2376,13 +2285,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -2393,13 +2302,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>39</v>
@@ -2407,13 +2316,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
@@ -2421,13 +2330,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
@@ -2435,13 +2344,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -2449,13 +2358,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -2463,99 +2372,373 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="F11" s="4">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="4">
+        <v>45188</v>
+      </c>
+    </row>
     <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
       <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="F18" s="4">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="4">
+        <v>44995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="B15" t="s">
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="4">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" t="s">
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="4">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="B29" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="B18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="16"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="16" t="s">
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>121</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" t="s">
-        <v>100</v>
+      <c r="C36" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quick update on my schedule progress
A update on progress in my schedule
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jjyoy\Documents\GitHubRepo\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D154D528-F17C-44E4-9C7B-86EC1AA5AB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D5C5AE-584F-4AF6-8B85-0C14FC404B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="600" windowWidth="14040" windowHeight="13635" tabRatio="731" firstSheet="2" activeTab="4" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="90" yWindow="1470" windowWidth="12375" windowHeight="11385" tabRatio="731" firstSheet="1" activeTab="1" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -1160,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1436,7 +1436,7 @@
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F17" s="4">
         <v>45188</v>
@@ -1456,7 +1456,7 @@
         <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F18" s="4">
         <v>45188</v>
@@ -1476,7 +1476,7 @@
         <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F19" s="4">
         <v>45188</v>
@@ -1496,7 +1496,7 @@
         <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="4">
         <v>45188</v>
@@ -1576,7 +1576,7 @@
         <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F24" s="4">
         <v>45188</v>
@@ -1596,7 +1596,7 @@
         <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F25" s="4">
         <v>45195</v>
@@ -1616,7 +1616,7 @@
         <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F26" s="4">
         <v>45195</v>
@@ -2229,7 +2229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C689EB-A68B-4BC4-B6BF-F1BC87CF5393}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove some of the stuff I add
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jjyoy\Documents\GitHubRepo\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\GitHub\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D5C5AE-584F-4AF6-8B85-0C14FC404B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB7AC42-034F-462B-B1CE-A7114913EA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1470" windowWidth="12375" windowHeight="11385" tabRatio="731" firstSheet="1" activeTab="1" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" firstSheet="1" activeTab="3" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="134">
   <si>
     <t>Footsteps</t>
   </si>
@@ -302,15 +302,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Design a Resource Room</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Design a Save Room</t>
-  </si>
-  <si>
     <t xml:space="preserve">Area 1 minimap </t>
   </si>
   <si>
@@ -472,9 +463,6 @@
   </si>
   <si>
     <t>Find &amp; Import pack</t>
-  </si>
-  <si>
-    <t>Transferred to Our Artist</t>
   </si>
   <si>
     <t>Player UI/ Looks</t>
@@ -996,10 +984,10 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1010,12 +998,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:2" ht="15.6">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="15.6">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1034,7 @@
     </row>
     <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1160,19 +1148,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1192,7 +1180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
@@ -1212,12 +1200,12 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1">
+    <row r="3" spans="1:6" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>37</v>
@@ -1232,7 +1220,7 @@
         <v>44998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+    <row r="4" spans="1:6" ht="15" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1252,7 +1240,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+    <row r="5" spans="1:6" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1272,7 +1260,7 @@
         <v>44991</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+    <row r="6" spans="1:6" ht="15" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1292,7 +1280,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+    <row r="7" spans="1:6" ht="15" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1312,7 +1300,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+    <row r="8" spans="1:6" ht="15" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -1332,7 +1320,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+    <row r="9" spans="1:6" ht="15" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1398,16 +1386,16 @@
     <row r="13" spans="1:6">
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+    <row r="14" spans="1:6" ht="15" thickBot="1"/>
+    <row r="15" spans="1:6" ht="15" thickBot="1">
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+    <row r="16" spans="1:6" ht="15" thickBot="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>37</v>
@@ -1422,12 +1410,12 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+    <row r="17" spans="1:8" ht="15" thickBot="1">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>37</v>
@@ -1442,12 +1430,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+    <row r="18" spans="1:8" ht="15" thickBot="1">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>37</v>
@@ -1462,12 +1450,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+    <row r="19" spans="1:8" ht="15" thickBot="1">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>37</v>
@@ -1482,12 +1470,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+    <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>37</v>
@@ -1502,12 +1490,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+    <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>37</v>
@@ -1522,18 +1510,18 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1">
+    <row r="22" spans="1:8" ht="15" thickBot="1">
       <c r="A22" t="s">
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
         <v>41</v>
@@ -1547,7 +1535,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>37</v>
@@ -1562,12 +1550,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1">
+    <row r="24" spans="1:8" ht="15" thickBot="1">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1582,12 +1570,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1">
+    <row r="25" spans="1:8" ht="15" thickBot="1">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>37</v>
@@ -1602,12 +1590,12 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1">
+    <row r="26" spans="1:8" ht="15" thickBot="1">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>37</v>
@@ -1622,12 +1610,12 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+    <row r="27" spans="1:8" ht="15" thickBot="1">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>37</v>
@@ -1642,19 +1630,19 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1">
+    <row r="28" spans="1:8" ht="15" thickBot="1">
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1">
+    <row r="29" spans="1:8" ht="15" thickBot="1">
       <c r="B29" s="11"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1">
+    <row r="30" spans="1:8" ht="15" thickBot="1">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>37</v>
@@ -1669,15 +1657,15 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1">
+    <row r="31" spans="1:8" ht="15" thickBot="1">
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1">
+    <row r="32" spans="1:8" ht="15" thickBot="1">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>37</v>
@@ -1693,12 +1681,12 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1">
+    <row r="33" spans="1:6" ht="15" thickBot="1">
       <c r="A33" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -1713,12 +1701,12 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
+    <row r="34" spans="1:6" ht="15" thickBot="1">
       <c r="A34" t="s">
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>37</v>
@@ -1733,12 +1721,12 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1">
+    <row r="35" spans="1:6" ht="15" thickBot="1">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>37</v>
@@ -1753,12 +1741,12 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1">
+    <row r="36" spans="1:6" ht="15" thickBot="1">
       <c r="A36" t="s">
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>37</v>
@@ -1773,33 +1761,33 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1">
+    <row r="37" spans="1:6" ht="15" thickBot="1">
       <c r="C37" s="6"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1">
+    <row r="38" spans="1:6" ht="15" thickBot="1"/>
+    <row r="39" spans="1:6" ht="15" thickBot="1">
       <c r="C39" s="6"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+    <row r="40" spans="1:6" ht="15" thickBot="1">
       <c r="C40" s="6"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1">
+    <row r="41" spans="1:6" ht="15" thickBot="1"/>
+    <row r="42" spans="1:6" ht="15" thickBot="1">
       <c r="C42" s="6"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1">
+    <row r="43" spans="1:6" ht="15" thickBot="1">
       <c r="C43" s="6"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1">
+    <row r="44" spans="1:6" ht="15" thickBot="1">
       <c r="C44" s="6"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1">
+    <row r="45" spans="1:6" ht="15" thickBot="1">
       <c r="C45" s="6"/>
       <c r="F45" s="4"/>
     </row>
@@ -1818,12 +1806,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1923,7 +1911,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1934,7 +1922,7 @@
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F12" s="4">
         <v>45181</v>
@@ -1948,7 +1936,7 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="4">
         <v>45181</v>
@@ -1977,18 +1965,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AABDC-3709-43B7-A9D3-19D374AE1A97}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2015,7 +2003,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -2027,12 +2015,12 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -2044,7 +2032,7 @@
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2061,7 +2049,7 @@
         <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2078,7 +2066,7 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2086,7 +2074,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -2095,7 +2083,7 @@
         <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2140,82 +2128,43 @@
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D17" t="s">
         <v>73</v>
       </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
+      <c r="E17" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2233,17 +2182,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="54.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2263,15 +2212,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6" ht="15" thickBot="1">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>39</v>
@@ -2285,13 +2234,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -2302,13 +2251,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
         <v>39</v>
@@ -2316,13 +2265,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
@@ -2330,13 +2279,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
@@ -2344,13 +2293,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -2358,13 +2307,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -2372,13 +2321,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
@@ -2386,13 +2335,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
         <v>43</v>
@@ -2408,10 +2357,10 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>
@@ -2428,10 +2377,10 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -2448,10 +2397,10 @@
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
@@ -2468,10 +2417,10 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -2488,10 +2437,10 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -2508,10 +2457,10 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -2530,10 +2479,10 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -2550,10 +2499,10 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
@@ -2567,10 +2516,10 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D21" t="s">
         <v>39</v>
@@ -2587,10 +2536,10 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
@@ -2607,10 +2556,10 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
@@ -2627,10 +2576,10 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
         <v>39</v>
@@ -2647,10 +2596,10 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
@@ -2661,26 +2610,26 @@
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="B28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2688,57 +2637,57 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated my part of the TLG Schedule
updated my part of the TLG Schedule
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\GitHub\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jjyoy\Documents\GitHubRepo\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB7AC42-034F-462B-B1CE-A7114913EA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9B85A9-C75E-4489-A7F9-B3EF15F0CFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" firstSheet="1" activeTab="3" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="731" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="131">
   <si>
     <t>Footsteps</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Area 4 minimap</t>
   </si>
   <si>
-    <t>Area 5 minimap</t>
-  </si>
-  <si>
     <t xml:space="preserve">Area 2 </t>
   </si>
   <si>
@@ -480,9 +477,6 @@
     <t>Area 4 skeleton</t>
   </si>
   <si>
-    <t>Area 5 skeleton</t>
-  </si>
-  <si>
     <t>Fix sticking to walls (ground check need to be changed.)</t>
   </si>
   <si>
@@ -493,9 +487,6 @@
   </si>
   <si>
     <t xml:space="preserve">Area 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area 5 </t>
   </si>
   <si>
     <t xml:space="preserve">Crates (breakable tiles but respawn when player leave room) </t>
@@ -980,14 +971,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1CC92-1BCB-4D56-BC10-E090CE41DC11}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -998,12 +989,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1034,7 +1025,7 @@
     </row>
     <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1148,19 +1139,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1171,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
@@ -1200,7 +1191,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -1220,7 +1211,7 @@
         <v>44998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1240,7 +1231,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1260,7 +1251,7 @@
         <v>44991</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1280,7 +1271,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1300,7 +1291,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -1320,7 +1311,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1386,11 +1377,11 @@
     <row r="13" spans="1:6">
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1"/>
-    <row r="15" spans="1:6" ht="15" thickBot="1">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1401,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1430,7 +1421,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1444,13 +1435,13 @@
         <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F18" s="4">
         <v>45188</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1464,33 +1455,17 @@
         <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F19" s="4">
         <v>45188</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="4">
-        <v>45188</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+      <c r="C20" s="6"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1510,7 +1485,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1521,7 +1496,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
         <v>41</v>
@@ -1535,7 +1510,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>37</v>
@@ -1550,12 +1525,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1">
+    <row r="24" spans="1:8" ht="15.75" thickBot="1">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1570,12 +1545,12 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>37</v>
@@ -1590,12 +1565,12 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>37</v>
@@ -1610,39 +1585,23 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="4">
-        <v>45195</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+      <c r="C27" s="6"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1">
       <c r="B29" s="11"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>37</v>
@@ -1657,15 +1616,15 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1">
+    <row r="32" spans="1:8" ht="15.75" thickBot="1">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>37</v>
@@ -1681,12 +1640,12 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1">
       <c r="A33" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -1695,18 +1654,18 @@
         <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F33" s="4">
         <v>45200</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1">
+    <row r="34" spans="1:6" ht="15.75" thickBot="1">
       <c r="A34" t="s">
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>37</v>
@@ -1715,18 +1674,18 @@
         <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F34" s="4">
         <v>45200</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1">
+    <row r="35" spans="1:6" ht="15.75" thickBot="1">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>37</v>
@@ -1735,59 +1694,43 @@
         <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F35" s="4">
         <v>45200</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" t="s">
-        <v>41</v>
-      </c>
-      <c r="F36" s="4">
-        <v>45200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C36" s="6"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1">
       <c r="C37" s="6"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1"/>
-    <row r="39" spans="1:6" ht="15" thickBot="1">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1">
       <c r="C39" s="6"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
       <c r="C40" s="6"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1"/>
-    <row r="42" spans="1:6" ht="15" thickBot="1">
+    <row r="41" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1">
       <c r="C42" s="6"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1">
       <c r="C43" s="6"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1">
+    <row r="44" spans="1:6" ht="15.75" thickBot="1">
       <c r="C44" s="6"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="15" thickBot="1">
+    <row r="45" spans="1:6" ht="15.75" thickBot="1">
       <c r="C45" s="6"/>
       <c r="F45" s="4"/>
     </row>
@@ -1806,12 +1749,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1911,7 +1854,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1922,7 +1865,7 @@
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F12" s="4">
         <v>45181</v>
@@ -1936,7 +1879,7 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F13" s="4">
         <v>45181</v>
@@ -1967,16 +1910,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AABDC-3709-43B7-A9D3-19D374AE1A97}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2003,7 +1946,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -2015,12 +1958,12 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -2032,7 +1975,7 @@
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2049,7 +1992,7 @@
         <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2066,7 +2009,7 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2074,7 +2017,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -2083,7 +2026,7 @@
         <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2130,15 +2073,15 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
         <v>54</v>
@@ -2147,15 +2090,15 @@
         <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
         <v>120</v>
-      </c>
-      <c r="B17" t="s">
-        <v>121</v>
       </c>
       <c r="C17" t="s">
         <v>54</v>
@@ -2164,7 +2107,7 @@
         <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2179,20 +2122,20 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="54.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2212,15 +2155,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>39</v>
@@ -2234,13 +2177,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -2251,13 +2194,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
         <v>39</v>
@@ -2265,13 +2208,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
@@ -2279,13 +2222,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
@@ -2293,13 +2236,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -2307,13 +2250,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -2321,13 +2264,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
@@ -2335,13 +2278,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
         <v>43</v>
@@ -2357,10 +2300,10 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>
@@ -2377,10 +2320,10 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -2397,10 +2340,10 @@
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
@@ -2417,10 +2360,10 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -2437,10 +2380,10 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -2457,10 +2400,10 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -2479,10 +2422,10 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -2499,10 +2442,10 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
@@ -2516,10 +2459,10 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
         <v>39</v>
@@ -2536,10 +2479,10 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
@@ -2556,10 +2499,10 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
@@ -2576,10 +2519,10 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
         <v>39</v>
@@ -2596,10 +2539,10 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
@@ -2609,27 +2552,36 @@
       </c>
     </row>
     <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
       <c r="B28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
         <v>103</v>
       </c>
-      <c r="C28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="B29" t="s">
-        <v>104</v>
-      </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2637,57 +2589,57 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added my updates to the TCG schedule
Added my updates to the TCG schedule
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\GitHub\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jjyoy\Documents\GitHubRepo\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4222AB71-0862-4B38-9261-BB884A8285D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A907B3-2AD6-429C-A083-58E00B37D3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="731" activeTab="3" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="731" activeTab="1" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="192">
   <si>
     <t>Footsteps</t>
   </si>
@@ -605,12 +605,101 @@
   <si>
     <t>Sprint not Listed in Controls</t>
   </si>
+  <si>
+    <t>Platform variation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (moving, falling, etc.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch objects </t>
+  </si>
+  <si>
+    <t xml:space="preserve">have a visual change when interacted with </t>
+  </si>
+  <si>
+    <t>explaining how to interact with the area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial </t>
+  </si>
+  <si>
+    <t>Map design</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> that differentiates each level.</t>
+  </si>
+  <si>
+    <t>More objects in the level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add some indicatory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">of the player direction. </t>
+  </si>
+  <si>
+    <t>Losing abilities after dying</t>
+  </si>
+  <si>
+    <t>(also fix sfx playing for ablility)</t>
+  </si>
+  <si>
+    <t>Getting stuck</t>
+  </si>
+  <si>
+    <t> in a wall or platform randomly</t>
+  </si>
+  <si>
+    <t>Some walls would not load in correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bypassing a large portion of the game. </t>
+  </si>
+  <si>
+    <t>Being able to grab items that you shouldn’t be able to</t>
+  </si>
+  <si>
+    <t>create a dead-end (need to be fixed)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inprovments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>More obstacles</t>
+  </si>
+  <si>
+    <t>Color change on interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health meter flashing with hit </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,6 +769,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -727,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -769,6 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,10 +1185,10 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1106,12 +1202,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.6">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.6">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1375,21 +1471,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1409,7 +1505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -1429,7 +1525,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
@@ -1449,7 +1545,7 @@
         <v>44998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -1469,7 +1565,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -1489,7 +1585,7 @@
         <v>44991</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1509,7 +1605,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -1529,7 +1625,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -1549,7 +1645,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
@@ -1615,11 +1711,11 @@
     <row r="13" spans="1:6">
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1"/>
-    <row r="15" spans="1:6" ht="15" thickBot="1">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1639,7 +1735,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1659,7 +1755,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1679,7 +1775,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1699,11 +1795,11 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="C20" s="6"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1723,7 +1819,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1763,7 +1859,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1">
+    <row r="24" spans="1:8" ht="15.75" thickBot="1">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1783,7 +1879,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1803,7 +1899,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1823,18 +1919,18 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
       <c r="C27" s="6"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1">
       <c r="B29" s="11"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1854,10 +1950,10 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1">
+    <row r="32" spans="1:8" ht="15.75" thickBot="1">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1878,7 +1974,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1898,7 +1994,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1">
+    <row r="34" spans="1:6" ht="15.75" thickBot="1">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1918,7 +2014,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1">
+    <row r="35" spans="1:6" ht="15.75" thickBot="1">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1938,39 +2034,242 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1">
       <c r="C36" s="6"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1">
+    <row r="37" spans="1:6" ht="15.75" thickBot="1">
       <c r="C37" s="6"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1"/>
-    <row r="39" spans="1:6" ht="15" thickBot="1">
-      <c r="C39" s="6"/>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>40</v>
+      </c>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1">
-      <c r="C40" s="6"/>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A40" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" t="s">
+        <v>172</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" t="s">
+        <v>40</v>
+      </c>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1"/>
-    <row r="42" spans="1:6" ht="15" thickBot="1">
-      <c r="C42" s="6"/>
+    <row r="41" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A41" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" t="s">
+        <v>40</v>
+      </c>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1">
-      <c r="C43" s="6"/>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>177</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" t="s">
+        <v>40</v>
+      </c>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1">
-      <c r="C44" s="6"/>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A44" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" t="s">
+        <v>40</v>
+      </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="15" thickBot="1">
-      <c r="C45" s="6"/>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A45" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" t="s">
+        <v>40</v>
+      </c>
       <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A46" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A48" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A51" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A52" t="s">
+        <v>190</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A53" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -1987,12 +2286,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2148,16 +2447,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AABDC-3709-43B7-A9D3-19D374AE1A97}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2579,17 +2878,17 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="54.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2609,7 +2908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Made changes to sound
Both in game and code. Not sure about this tile factory so I hope I dont break anything. Also updated some of my beta tasks to done.
</commit_message>
<xml_diff>
--- a/TLG Schedule.xlsx
+++ b/TLG Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jjyoy\Documents\GitHubRepo\Total-Let-Down-Games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4TaL\Desktop\School Semesters\Fall 2023\489GIT\Total-Let-Down-Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A907B3-2AD6-429C-A083-58E00B37D3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBFF94B-755A-48A5-AAC0-834B8293F8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="731" activeTab="1" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="731" xr2:uid="{A6E805F7-2F73-4FA8-A456-AF61C7F2897D}"/>
   </bookViews>
   <sheets>
     <sheet name="Marcus Queiro(Sound Effects)" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="192">
   <si>
     <t>Footsteps</t>
   </si>
@@ -1181,14 +1181,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1CC92-1BCB-4D56-BC10-E090CE41DC11}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="66" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1202,12 +1202,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15.5">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15.5">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:3" ht="20.149999999999999" customHeight="1">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -1442,6 +1442,9 @@
       <c r="A33" t="s">
         <v>142</v>
       </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
       <c r="C33" t="s">
         <v>152</v>
       </c>
@@ -1457,6 +1460,9 @@
     <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>143</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
       </c>
       <c r="C35" t="s">
         <v>152</v>
@@ -1473,19 +1479,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0CBB7-90BA-4370-8BA1-B84CEA81385B}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1505,7 +1511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -1525,7 +1531,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1">
+    <row r="3" spans="1:6" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
@@ -1545,7 +1551,7 @@
         <v>44998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+    <row r="4" spans="1:6" ht="15" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+    <row r="5" spans="1:6" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>44991</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+    <row r="6" spans="1:6" ht="15" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>45033</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+    <row r="7" spans="1:6" ht="15" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -1625,7 +1631,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+    <row r="8" spans="1:6" ht="15" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+    <row r="9" spans="1:6" ht="15" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
@@ -1711,11 +1717,11 @@
     <row r="13" spans="1:6">
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+    <row r="14" spans="1:6" ht="15" thickBot="1"/>
+    <row r="15" spans="1:6" ht="15" thickBot="1">
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+    <row r="16" spans="1:6" ht="15" thickBot="1">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+    <row r="17" spans="1:8" ht="15" thickBot="1">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1755,7 +1761,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+    <row r="18" spans="1:8" ht="15" thickBot="1">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+    <row r="19" spans="1:8" ht="15" thickBot="1">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1795,11 +1801,11 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+    <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="C20" s="6"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+    <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1">
+    <row r="22" spans="1:8" ht="15" thickBot="1">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1">
+    <row r="24" spans="1:8" ht="15" thickBot="1">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1">
+    <row r="25" spans="1:8" ht="15" thickBot="1">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1899,7 +1905,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1">
+    <row r="26" spans="1:8" ht="15" thickBot="1">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1919,18 +1925,18 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+    <row r="27" spans="1:8" ht="15" thickBot="1">
       <c r="C27" s="6"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1">
+    <row r="28" spans="1:8" ht="15" thickBot="1">
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1">
+    <row r="29" spans="1:8" ht="15" thickBot="1">
       <c r="B29" s="11"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1">
+    <row r="30" spans="1:8" ht="15" thickBot="1">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1950,10 +1956,10 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1">
+    <row r="31" spans="1:8" ht="15" thickBot="1">
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1">
+    <row r="32" spans="1:8" ht="15" thickBot="1">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1974,7 +1980,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1">
+    <row r="33" spans="1:6" ht="15" thickBot="1">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
+    <row r="34" spans="1:6" ht="15" thickBot="1">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1">
+    <row r="35" spans="1:6" ht="15" thickBot="1">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2034,11 +2040,11 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1">
+    <row r="36" spans="1:6" ht="15" thickBot="1">
       <c r="C36" s="6"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1">
+    <row r="37" spans="1:6" ht="15" thickBot="1">
       <c r="C37" s="6"/>
       <c r="F37" s="4"/>
     </row>
@@ -2065,7 +2071,7 @@
       </c>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+    <row r="40" spans="1:6" ht="15" thickBot="1">
       <c r="A40" t="s">
         <v>171</v>
       </c>
@@ -2083,7 +2089,7 @@
       </c>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1">
+    <row r="41" spans="1:6" ht="15" thickBot="1">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1">
+    <row r="42" spans="1:6" ht="15" thickBot="1">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -2133,7 +2139,7 @@
       </c>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1">
+    <row r="44" spans="1:6" ht="15" thickBot="1">
       <c r="A44" t="s">
         <v>178</v>
       </c>
@@ -2151,7 +2157,7 @@
       </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1">
+    <row r="45" spans="1:6" ht="15" thickBot="1">
       <c r="A45" t="s">
         <v>180</v>
       </c>
@@ -2169,7 +2175,7 @@
       </c>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1">
+    <row r="46" spans="1:6" ht="15" thickBot="1">
       <c r="A46" t="s">
         <v>182</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1">
+    <row r="48" spans="1:6" ht="15" thickBot="1">
       <c r="A48" t="s">
         <v>184</v>
       </c>
@@ -2220,16 +2226,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+    <row r="49" spans="1:5" ht="15" thickBot="1">
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1">
+    <row r="50" spans="1:5" ht="15" thickBot="1">
       <c r="A50" t="s">
         <v>188</v>
       </c>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1">
+    <row r="51" spans="1:5" ht="15" thickBot="1">
       <c r="A51" s="17" t="s">
         <v>189</v>
       </c>
@@ -2243,7 +2249,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1">
+    <row r="52" spans="1:5" ht="15" thickBot="1">
       <c r="A52" t="s">
         <v>190</v>
       </c>
@@ -2257,7 +2263,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1">
+    <row r="53" spans="1:5" ht="15" thickBot="1">
       <c r="A53" s="17" t="s">
         <v>191</v>
       </c>
@@ -2286,12 +2292,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2451,12 +2457,12 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2878,17 +2884,17 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="54.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2908,7 +2914,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6" ht="15" thickBot="1">
       <c r="A2" t="s">
         <v>89</v>
       </c>

</xml_diff>